<commit_message>
added, modified new files
</commit_message>
<xml_diff>
--- a/transactions.xlsx
+++ b/transactions.xlsx
@@ -1465,8 +1465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A1090" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E1114" sqref="E1114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1476,7 +1476,7 @@
     <col min="3" max="3" width="14.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" style="12" customWidth="1"/>
     <col min="5" max="5" width="68.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="22" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -23710,13 +23710,13 @@
         <v>6</v>
       </c>
       <c r="D1112" s="7" t="s">
-        <v>308</v>
+        <v>38</v>
       </c>
       <c r="E1112" s="7" t="s">
         <v>307</v>
       </c>
       <c r="F1112" s="3">
-        <v>4580</v>
+        <v>-4580</v>
       </c>
     </row>
     <row r="1113" spans="1:6" x14ac:dyDescent="0.25">
@@ -23730,13 +23730,13 @@
         <v>6</v>
       </c>
       <c r="D1113" s="7" t="s">
-        <v>216</v>
+        <v>38</v>
       </c>
       <c r="E1113" s="7" t="s">
         <v>309</v>
       </c>
       <c r="F1113" s="3">
-        <v>3500</v>
+        <v>-3500</v>
       </c>
     </row>
     <row r="1114" spans="1:6" x14ac:dyDescent="0.25">
@@ -23750,13 +23750,13 @@
         <v>6</v>
       </c>
       <c r="D1114" s="7" t="s">
-        <v>38</v>
+        <v>308</v>
       </c>
       <c r="E1114" s="7" t="s">
         <v>307</v>
       </c>
       <c r="F1114" s="3">
-        <v>-4580</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="1115" spans="1:6" x14ac:dyDescent="0.25">
@@ -23770,13 +23770,13 @@
         <v>6</v>
       </c>
       <c r="D1115" s="7" t="s">
-        <v>38</v>
+        <v>216</v>
       </c>
       <c r="E1115" s="7" t="s">
         <v>309</v>
       </c>
       <c r="F1115" s="3">
-        <v>-3500</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="1116" spans="1:6" x14ac:dyDescent="0.25">
@@ -23790,13 +23790,13 @@
         <v>6</v>
       </c>
       <c r="D1116" s="7" t="s">
-        <v>350</v>
+        <v>38</v>
       </c>
       <c r="E1116" s="7" t="s">
         <v>351</v>
       </c>
       <c r="F1116" s="3">
-        <v>3963</v>
+        <v>-3963</v>
       </c>
     </row>
     <row r="1117" spans="1:6" x14ac:dyDescent="0.25">
@@ -23810,13 +23810,13 @@
         <v>6</v>
       </c>
       <c r="D1117" s="7" t="s">
-        <v>308</v>
+        <v>38</v>
       </c>
       <c r="E1117" s="7" t="s">
         <v>307</v>
       </c>
       <c r="F1117" s="3">
-        <v>4095</v>
+        <v>-4095</v>
       </c>
     </row>
     <row r="1118" spans="1:6" x14ac:dyDescent="0.25">
@@ -23830,13 +23830,13 @@
         <v>6</v>
       </c>
       <c r="D1118" s="7" t="s">
-        <v>38</v>
+        <v>308</v>
       </c>
       <c r="E1118" s="7" t="s">
         <v>307</v>
       </c>
       <c r="F1118" s="3">
-        <v>-4095</v>
+        <v>4095</v>
       </c>
     </row>
     <row r="1119" spans="1:6" x14ac:dyDescent="0.25">
@@ -23850,13 +23850,13 @@
         <v>6</v>
       </c>
       <c r="D1119" s="7" t="s">
-        <v>38</v>
+        <v>350</v>
       </c>
       <c r="E1119" s="7" t="s">
         <v>351</v>
       </c>
       <c r="F1119" s="3">
-        <v>-3963</v>
+        <v>3963</v>
       </c>
     </row>
     <row r="1120" spans="1:6" x14ac:dyDescent="0.25">
@@ -23870,13 +23870,13 @@
         <v>6</v>
       </c>
       <c r="D1120" s="7" t="s">
-        <v>216</v>
+        <v>38</v>
       </c>
       <c r="E1120" s="7" t="s">
         <v>309</v>
       </c>
       <c r="F1120" s="3">
-        <v>3500</v>
+        <v>-3500</v>
       </c>
     </row>
     <row r="1121" spans="1:6" x14ac:dyDescent="0.25">
@@ -23890,13 +23890,13 @@
         <v>6</v>
       </c>
       <c r="D1121" s="7" t="s">
-        <v>308</v>
+        <v>38</v>
       </c>
       <c r="E1121" s="7" t="s">
         <v>307</v>
       </c>
       <c r="F1121" s="3">
-        <v>2300</v>
+        <v>-2300</v>
       </c>
     </row>
     <row r="1122" spans="1:6" x14ac:dyDescent="0.25">
@@ -23910,13 +23910,13 @@
         <v>6</v>
       </c>
       <c r="D1122" s="7" t="s">
-        <v>38</v>
+        <v>216</v>
       </c>
       <c r="E1122" s="7" t="s">
         <v>309</v>
       </c>
       <c r="F1122" s="3">
-        <v>-3500</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="1123" spans="1:6" x14ac:dyDescent="0.25">
@@ -23970,13 +23970,13 @@
         <v>6</v>
       </c>
       <c r="D1125" s="7" t="s">
-        <v>38</v>
+        <v>308</v>
       </c>
       <c r="E1125" s="7" t="s">
         <v>307</v>
       </c>
       <c r="F1125" s="3">
-        <v>-2300</v>
+        <v>2300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>